<commit_message>
Done the wk04's task - Linyi
</commit_message>
<xml_diff>
--- a/Planning and Execution/Phython_GUI_Capstone_Planning_and_Progress_2018.xlsx
+++ b/Planning and Execution/Phython_GUI_Capstone_Planning_and_Progress_2018.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
   <si>
     <t>Priority #</t>
   </si>
@@ -1055,7 +1055,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1380,7 +1380,9 @@
       <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
         <v>88</v>
@@ -1480,7 +1482,9 @@
       <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
         <v>88</v>

</xml_diff>